<commit_message>
Add support for alternate category import #1906
</commit_message>
<xml_diff>
--- a/module/Application/test/data/import_jmp.xlsx
+++ b/module/Application/test/data/import_jmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="470" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="942" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables_W" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="171">
+  <si>
+    <t>Survey Category</t>
+  </si>
   <si>
     <t>Code 1</t>
   </si>
@@ -286,6 +289,9 @@
     <t>Cat 4-32</t>
   </si>
   <si>
+    <t>B Survey Category</t>
+  </si>
+  <si>
     <t>Code 3</t>
   </si>
   <si>
@@ -319,6 +325,9 @@
     <t>B Cat 1-5</t>
   </si>
   <si>
+    <t>Alternate B Category 2</t>
+  </si>
+  <si>
     <t>B Category 2</t>
   </si>
   <si>
@@ -326,6 +335,9 @@
   </si>
   <si>
     <t>B Cat 2-2</t>
+  </si>
+  <si>
+    <t>Alternate B Cat 2-3</t>
   </si>
   <si>
     <t>B Cat 2-3</t>
@@ -619,25 +631,31 @@
   </sheetPr>
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2039215686275"/>
-    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="15.1490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3058823529412"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="15.2235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>1</v>
-      </c>
       <c r="I1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1" s="0" t="str">
         <f aca="false">$D$1</f>
@@ -646,10 +664,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -662,39 +680,39 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="L4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -709,7 +727,7 @@
         <v>6.6</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>60</v>
@@ -723,7 +741,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -738,7 +756,7 @@
         <v>4.3</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J6" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J7),ISNUMBER(J8)),SUM(J7,J8),"")</f>
@@ -755,10 +773,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -770,26 +788,26 @@
         <v>4.3</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -801,23 +819,23 @@
         <v>2.3</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
@@ -832,7 +850,7 @@
         <v>74.6</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J11" s="0" t="n">
         <f aca="false">IF(SUMIF(G12:G53,"&gt;""",J12:J53)=0,"",SUMIF(G12:G53,"&gt;""",J12:J53))</f>
@@ -849,7 +867,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
@@ -864,7 +882,7 @@
         <v>66.6</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" s="0" t="n">
         <f aca="false">IF(SUMIF(G14:G17,"&gt;""",J14:J17)+SUMIF(G26:G29,"&gt;""",J26:J29)+SUMIF(G46:G49,"&gt;""",J46:J49)+SUMIF(G34:G37,"&gt;""",J34:J37)=0,"",SUMIF(G14:G17,"&gt;""",J14:J17)+SUMIF(G26:G29,"&gt;""",J26:J29)+SUMIF(G46:G49,"&gt;""",J46:J49)+SUMIF(G34:G37,"&gt;""",J34:J37))</f>
@@ -881,7 +899,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -896,7 +914,7 @@
         <v/>
       </c>
       <c r="I13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J13" s="0" t="str">
         <f aca="false">IF(SUMIF(G18:G21,"&gt;""",J18:J21)+SUMIF(G38:G41,"&gt;""",J38:J41)+SUMIF(G50:G53,"&gt;""",J50:J53)=0,"",SUMIF(G18:G21,"&gt;""",J18:J21)+SUMIF(G38:G41,"&gt;""",J38:J41)+SUMIF(G50:G53,"&gt;""",J50:J53))</f>
@@ -913,7 +931,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="C14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -928,7 +946,7 @@
         <v>66.6</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(G26),ISTEXT(G34),ISTEXT(G46)),SUM(J26,J34,J46),IF(OR(ISNUMBER(J15),ISNUMBER(J16),ISNUMBER(J17)),SUM(J15,J16,J17),""))</f>
@@ -945,7 +963,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -960,7 +978,7 @@
         <v/>
       </c>
       <c r="I15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J27),ISNUMBER(J35),ISNUMBER(J47)),SUM(J27,J35,J47),"")</f>
@@ -977,7 +995,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -992,7 +1010,7 @@
         <v/>
       </c>
       <c r="I16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J36),ISNUMBER(J48)),SUM(J28,J36,J48),"")</f>
@@ -1009,7 +1027,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -1024,7 +1042,7 @@
         <v/>
       </c>
       <c r="I17" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J37),ISNUMBER(J49)),SUM(J29,J37,J49),"")</f>
@@ -1041,7 +1059,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -1056,7 +1074,7 @@
         <v/>
       </c>
       <c r="I18" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G38),ISTEXT(G50)),SUM(J38,J50),IF(OR(ISNUMBER(J19),ISNUMBER(J20),ISNUMBER(J21)),SUM(J19,J20,J21),""))</f>
@@ -1073,7 +1091,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -1088,7 +1106,7 @@
         <v/>
       </c>
       <c r="I19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J39),ISNUMBER(J51)),SUM(J39,J51),"")</f>
@@ -1105,7 +1123,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -1120,7 +1138,7 @@
         <v/>
       </c>
       <c r="I20" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J40),ISNUMBER(J52)),SUM(J40,J52),"")</f>
@@ -1137,7 +1155,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -1152,7 +1170,7 @@
         <v/>
       </c>
       <c r="I21" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J41),ISNUMBER(J53)),SUM(J41,J53),"")</f>
@@ -1169,10 +1187,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J22" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J23),ISNUMBER(J24),ISNUMBER(J25),ISNUMBER(J26),ISNUMBER(J27),ISNUMBER(J28),ISNUMBER(J29),ISNUMBER(J30),ISNUMBER(J31),ISNUMBER(J32),ISNUMBER(J33),ISNUMBER(J34),ISNUMBER(J35),ISNUMBER(J36),ISNUMBER(J37),ISNUMBER(J38),ISNUMBER(J39),ISNUMBER(J40),ISNUMBER(J41)),SUMIF(G23:G41,"&gt;""",J23:J41),"")</f>
@@ -1189,7 +1207,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -1204,7 +1222,7 @@
         <v/>
       </c>
       <c r="I23" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J27),ISNUMBER(J31)),SUM(J27,J31),"")</f>
@@ -1221,7 +1239,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -1236,7 +1254,7 @@
         <v/>
       </c>
       <c r="I24" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J28),ISNUMBER(J32)),SUM(J28,J32),"")</f>
@@ -1253,7 +1271,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -1268,7 +1286,7 @@
         <v/>
       </c>
       <c r="I25" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J29),ISNUMBER(J33)),SUM(J29,J33),"")</f>
@@ -1285,10 +1303,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -1300,10 +1318,10 @@
         <v>66.6</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>22</v>
@@ -1317,34 +1335,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -1356,10 +1374,10 @@
         <v>8</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>1</v>
@@ -1373,7 +1391,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -1388,7 +1406,7 @@
         <v/>
       </c>
       <c r="I31" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J35),ISNUMBER(J39)),SUM(J35,J39),"")</f>
@@ -1405,7 +1423,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -1420,7 +1438,7 @@
         <v/>
       </c>
       <c r="I32" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J36),ISNUMBER(J40)),SUM(J36,J40),"")</f>
@@ -1437,7 +1455,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -1452,7 +1470,7 @@
         <v/>
       </c>
       <c r="I33" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J37),ISNUMBER(J41)),SUM(J37,J41),"")</f>
@@ -1469,7 +1487,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -1484,7 +1502,7 @@
         <v/>
       </c>
       <c r="I34" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G35),ISTEXT(G36),ISTEXT(G37)),SUM(J35,J36,J37),"")</f>
@@ -1501,31 +1519,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -1540,7 +1558,7 @@
         <v/>
       </c>
       <c r="I38" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G39),ISTEXT(G40),ISTEXT(G41)),SUM(J39,J40,J41),"")</f>
@@ -1557,31 +1575,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -1596,7 +1614,7 @@
         <v/>
       </c>
       <c r="I42" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J43),ISNUMBER(J44),ISNUMBER(J45),ISNUMBER(J46),ISNUMBER(J47),ISNUMBER(J48),ISNUMBER(J49),ISNUMBER(J50),ISNUMBER(J51),ISNUMBER(J52),ISNUMBER(J53)),SUMIF(G43:G53,"&gt;""",J43:J53),"")</f>
@@ -1613,7 +1631,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -1628,7 +1646,7 @@
         <v/>
       </c>
       <c r="I43" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J47),ISNUMBER(J51)),SUM(J47,J51),"")</f>
@@ -1645,7 +1663,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -1660,7 +1678,7 @@
         <v/>
       </c>
       <c r="H44" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J48),ISNUMBER(J52)),SUM(J48,J52),"")</f>
@@ -1677,7 +1695,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -1688,7 +1706,7 @@
         <v/>
       </c>
       <c r="I45" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(K49),ISNUMBER(K53)),SUM(K49,K53),"")</f>
@@ -1701,7 +1719,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -1716,7 +1734,7 @@
         <v/>
       </c>
       <c r="I46" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G47),ISTEXT(G48),ISTEXT(G49)),SUM(J47,J48,J49),"")</f>
@@ -1733,31 +1751,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -1772,7 +1790,7 @@
         <v/>
       </c>
       <c r="I50" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(G51),ISTEXT(G52),ISTEXT(G53)),SUM(J51,J52,J53),"")</f>
@@ -1789,31 +1807,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -1828,7 +1846,7 @@
         <v/>
       </c>
       <c r="I54" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J55),ISNUMBER(J56)),SUM(J55,J56),"")</f>
@@ -1845,23 +1863,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -1876,7 +1894,7 @@
         <v/>
       </c>
       <c r="I57" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J58),ISNUMBER(J59)),SUM(J58,J59),"")</f>
@@ -1893,23 +1911,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -1924,7 +1942,7 @@
         <v>9.8</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J60" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J61),ISNUMBER(J62),ISNUMBER(J63),ISNUMBER(J64),ISNUMBER(J65),ISNUMBER(J66),ISNUMBER(J67)),SUM(J61:J67),"")</f>
@@ -1941,10 +1959,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -1956,31 +1974,31 @@
         <v>7</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -1992,36 +2010,36 @@
         <v>2.8</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -2036,7 +2054,7 @@
         <v/>
       </c>
       <c r="I68" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(J69),ISNUMBER(J70)),SUM(J69,J70),"")</f>
@@ -2053,23 +2071,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -2084,7 +2102,7 @@
         <v>0.1</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J72),ISNUMBER(J73),ISNUMBER(J74),ISNUMBER(J75)),SUM(J72:J75),"")</f>
@@ -2101,23 +2119,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -2129,7 +2147,7 @@
         <v>0.1</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J74" s="0" t="n">
         <v>5</v>
@@ -2143,15 +2161,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -2163,12 +2181,12 @@
         <v>0.1</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="B77" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D5),ISNUMBER(D11),ISNUMBER(D54),ISNUMBER(D57),ISNUMBER(D60),ISNUMBER(D71),ISNUMBER(D76)),SUM(D5,D11,D54,D57,D60,D68,D71,D76),"")</f>
@@ -2183,7 +2201,7 @@
         <v>91.2</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(J5),ISNUMBER(J11),ISNUMBER(J54),ISNUMBER(J57),ISNUMBER(J60),ISNUMBER(J71),ISNUMBER(J76)),SUM(J5,J11,J54,J57,J60,J68,J71,J76),"")</f>
@@ -2216,27 +2234,30 @@
   </sheetPr>
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="G1 A2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2039215686275"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="15.1490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="15.2235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>88</v>
+      </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
@@ -2246,24 +2267,24 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="B5" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D6),ISNUMBER(D9),ISNUMBER(D10)),SUM(D6,D9,D10),"")</f>
@@ -2280,7 +2301,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="C6" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D7),ISNUMBER(D8)),SUM(D7,D8),"")</f>
@@ -2297,10 +2318,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>23.1</v>
@@ -2314,15 +2335,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>7</v>
@@ -2336,46 +2357,49 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="C10" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
+        <v>100</v>
+      </c>
       <c r="B11" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",D12:D53)=0,"",SUMIF(A12:A53,"&gt;""",D12:D53))</f>
-        <v>50.4</v>
+        <v>95.4</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",E12:E53)=0,"",SUMIF(A12:A53,"&gt;""",E12:E53))</f>
-        <v>91.3</v>
+        <v>176.3</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">IF(SUMIF(A12:A53,"&gt;""",F12:F53)=0,"",SUMIF(A12:A53,"&gt;""",F12:F53))</f>
-        <v>74.6</v>
+        <v>141.2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="C12" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37)=0,"",SUMIF(A14:A17,"&gt;""",D14:D17)+SUMIF(A26:A29,"&gt;""",D26:D29)+SUMIF(A46:A49,"&gt;""",D46:D49)+SUMIF(A34:A37,"&gt;""",D34:D37))</f>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",E14:E17)+SUMIF(A26:A29,"&gt;""",E26:E29)+SUMIF(A46:A49,"&gt;""",E46:E49)+SUMIF(A34:A37,"&gt;""",E34:E37)=0,"",SUMIF(A14:A17,"&gt;""",E14:E17)+SUMIF(A26:A29,"&gt;""",E26:E29)+SUMIF(A46:A49,"&gt;""",E46:E49)+SUMIF(A34:A37,"&gt;""",E34:E37))</f>
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">IF(SUMIF(A14:A17,"&gt;""",F14:F17)+SUMIF(A26:A29,"&gt;""",F26:F29)+SUMIF(A46:A49,"&gt;""",F46:F49)+SUMIF(A34:A37,"&gt;""",F34:F37)=0,"",SUMIF(A14:A17,"&gt;""",F14:F17)+SUMIF(A26:A29,"&gt;""",F26:F29)+SUMIF(A46:A49,"&gt;""",F46:F49)+SUMIF(A34:A37,"&gt;""",F34:F37))</f>
-        <v>66.6</v>
+        <v>133.2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D13" s="0" t="str">
         <f aca="false">IF(SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53)=0,"",SUMIF(A18:A21,"&gt;""",D18:D21)+SUMIF(A38:A41,"&gt;""",D38:D41)+SUMIF(A50:A53,"&gt;""",D50:D53))</f>
@@ -2391,8 +2415,11 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="14">
+      <c r="A14" s="0" t="s">
+        <v>104</v>
+      </c>
       <c r="C14" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISTEXT(A26),ISTEXT(A34),ISTEXT(A46)),SUM(D26,D34,D46),IF(OR(ISNUMBER(D15),ISNUMBER(D16),ISNUMBER(D17)),SUM(D15,D16,D17),""))</f>
@@ -2409,7 +2436,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D15" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D35),ISNUMBER(D47)),SUM(D27,D35,D47),"")</f>
@@ -2426,7 +2453,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D16" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D36),ISNUMBER(D48)),SUM(D28,D36,D48),"")</f>
@@ -2443,7 +2470,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="C17" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D17" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D37),ISNUMBER(D49)),SUM(D29,D37,D49),"")</f>
@@ -2460,7 +2487,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="C18" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D18" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A38),ISTEXT(A50)),SUM(D38,D50),IF(OR(ISNUMBER(D19),ISNUMBER(D20),ISNUMBER(D21)),SUM(D19,D20,D21),""))</f>
@@ -2477,7 +2504,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D19" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D39),ISNUMBER(D51)),SUM(D39,D51),"")</f>
@@ -2494,7 +2521,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D20" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D40),ISNUMBER(D52)),SUM(D40,D52),"")</f>
@@ -2511,7 +2538,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D21" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D41),ISNUMBER(D53)),SUM(D41,D53),"")</f>
@@ -2528,12 +2555,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="C23" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D23" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D27),ISNUMBER(D31)),SUM(D27,D31),"")</f>
@@ -2550,7 +2577,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="24">
       <c r="C24" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D24" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D28),ISNUMBER(D32)),SUM(D28,D32),"")</f>
@@ -2567,7 +2594,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="25">
       <c r="C25" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D25" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D29),ISNUMBER(D33)),SUM(D29,D33),"")</f>
@@ -2584,10 +2611,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>45</v>
@@ -2601,25 +2628,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="27">
       <c r="C27" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="28">
       <c r="C28" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="C29" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>5.4</v>
@@ -2633,7 +2660,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="C31" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D31" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D35),ISNUMBER(D39)),SUM(D35,D39),"")</f>
@@ -2650,7 +2677,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="C32" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D32" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D36),ISNUMBER(D40)),SUM(D36,D40),"")</f>
@@ -2667,7 +2694,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="C33" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D33" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D37),ISNUMBER(D41)),SUM(D37,D41),"")</f>
@@ -2684,7 +2711,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="C34" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D34" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A35),ISTEXT(A36),ISTEXT(A37)),SUM(D35,D36,D37),"")</f>
@@ -2701,22 +2728,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="C35" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="C36" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="C37" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="C38" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D38" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A39),ISTEXT(A40),ISTEXT(A41)),SUM(D39,D40,D41),"")</f>
@@ -2733,22 +2760,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="C39" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="C40" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="C41" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="C42" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D42" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D43),ISNUMBER(D44),ISNUMBER(D45),ISNUMBER(D46),ISNUMBER(D47),ISNUMBER(D48),ISNUMBER(D49),ISNUMBER(D50),ISNUMBER(D51),ISNUMBER(D52),ISNUMBER(D53)),SUMIF(A43:A53,"&gt;""",D43:D53),"")</f>
@@ -2765,7 +2792,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="C43" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D43" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D47),ISNUMBER(D51)),SUM(D47,D51),"")</f>
@@ -2782,7 +2809,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="B44" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D44" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D48),ISNUMBER(D52)),SUM(D48,D52),"")</f>
@@ -2799,7 +2826,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="C45" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E45" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(E49),ISNUMBER(E53)),SUM(E49,E53),"")</f>
@@ -2812,7 +2839,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="C46" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D46" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A47),ISTEXT(A48),ISTEXT(A49)),SUM(D47,D48,D49),"")</f>
@@ -2829,22 +2856,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="C47" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="48">
       <c r="C48" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="49">
       <c r="C49" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="50">
       <c r="C50" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D50" s="0" t="str">
         <f aca="false">IF(OR(ISTEXT(A51),ISTEXT(A52),ISTEXT(A53)),SUM(D51,D52,D53),"")</f>
@@ -2861,22 +2888,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="51">
       <c r="C51" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D54" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D55),ISNUMBER(D56)),SUM(D55,D56),"")</f>
@@ -2893,17 +2920,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="57">
       <c r="C57" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D57" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D58),ISNUMBER(D59)),SUM(D58,D59),"")</f>
@@ -2920,17 +2947,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="59">
       <c r="C59" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D60" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D61),ISNUMBER(D62),ISNUMBER(D63),ISNUMBER(D64),ISNUMBER(D65),ISNUMBER(D66),ISNUMBER(D67)),SUM(D61:D67),"")</f>
@@ -2947,10 +2974,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>7</v>
@@ -2964,17 +2991,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="63">
       <c r="C63" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="64">
       <c r="C64" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>4</v>
@@ -2988,22 +3015,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="68">
       <c r="C68" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D68" s="0" t="str">
         <f aca="false">IF(OR(ISNUMBER(D69),ISNUMBER(D70)),SUM(D69,D70),"")</f>
@@ -3020,17 +3047,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="69">
       <c r="C69" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="70">
       <c r="C70" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="71">
       <c r="C71" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D71" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D72),ISNUMBER(D73),ISNUMBER(D74),ISNUMBER(D75)),SUM(D72:D75),"")</f>
@@ -3047,17 +3074,17 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="72">
       <c r="C72" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="73">
       <c r="C73" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="74">
       <c r="C74" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>8.5</v>
@@ -3071,12 +3098,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="75">
       <c r="C75" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>0</v>
@@ -3090,19 +3117,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="77">
       <c r="B77" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(D5),ISNUMBER(D11),ISNUMBER(D54),ISNUMBER(D57),ISNUMBER(D60),ISNUMBER(D71),ISNUMBER(D76)),SUM(D5,D11,D54,D57,D60,D68,D71,D76),"")</f>
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="E77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(E5),ISNUMBER(E11),ISNUMBER(E54),ISNUMBER(E57),ISNUMBER(E60),ISNUMBER(E71),ISNUMBER(E76)),SUM(E5,E11,E54,E57,E60,E68,E71,E76),"")</f>
-        <v>98.9</v>
+        <v>183.9</v>
       </c>
       <c r="F77" s="0" t="n">
         <f aca="false">IF(OR(ISNUMBER(F5),ISNUMBER(F11),ISNUMBER(F54),ISNUMBER(F57),ISNUMBER(F60),ISNUMBER(F71),ISNUMBER(F76)),SUM(F5,F11,F54,F57,F60,F68,F71,F76),"")</f>
-        <v>91.2</v>
+        <v>157.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>